<commit_message>
Update DPE to correct errors
correct a incorrect parenthesis and an incorrect variable name (pm_weight, the correct one is Weight)
</commit_message>
<xml_diff>
--- a/data_processing_elements-MSN.xlsx
+++ b/data_processing_elements-MSN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlaforme\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD14D21D-497B-487D-96BD-22DE88C0F415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96F28E5-5F30-4416-8EB0-E7A42A419969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1161,9 +1161,6 @@
     <t>BPM</t>
   </si>
   <si>
-    <t>N_Wmax_combined</t>
-  </si>
-  <si>
     <t>N_Wmax_combined is based on heart rate (HR) values if test was terminated on HR; based on Rate of Perceived Exertion (RPE) values if test was terminated based on RPE.</t>
   </si>
   <si>
@@ -1570,9 +1567,6 @@
 https://pubmed.ncbi.nlm.nih.gov/17331263/</t>
   </si>
   <si>
-    <t>round((13.895 * N_Wmax_combined + 151) / pm_weight, 2)</t>
-  </si>
-  <si>
     <t>case_when(
 !is.na(Tot_chol) &amp; !is.na(HDL) &amp; !is.na(Triglyc) ~ round(Tot_chol - HDL - (Triglyc/2.2), 2); 
 ELSE ~ NA_real_)</t>
@@ -1601,8 +1595,14 @@
 temp_SF36_Q12 = if_else(!SF36_Q12 %in% c(1, 2, 3), NA, 1)) %&gt;%
 select(temp_SF36_Q03, temp_SF36_Q04, temp_SF36_Q05, temp_SF36_Q06, temp_SF36_Q07,
 temp_SF36_Q08, temp_SF36_Q09, temp_SF36_Q10, temp_SF36_Q11, temp_SF36_Q12),
-na.rm=TRUE)) %&gt;%
+na.rm=TRUE) %&gt;%
 mutate(phy_SF36_nb_items = if_else(phy_SF36_nb_items == 0, NA, phy_SF36_nb_items))</t>
+  </si>
+  <si>
+    <t>round((13.895 * N_Wmax_combined + 151) / Weight, 2)</t>
+  </si>
+  <si>
+    <t>N_Wmax_combined;Weight</t>
   </si>
 </sst>
 </file>
@@ -2098,10 +2098,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2124,7 @@
     <col min="16" max="16" width="12.7109375" style="14" customWidth="1"/>
     <col min="17" max="17" width="12.42578125" style="14" customWidth="1"/>
     <col min="18" max="18" width="17.5703125" style="14" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="14" customWidth="1"/>
+    <col min="19" max="19" width="119.5703125" style="14" customWidth="1"/>
     <col min="20" max="21" width="9.140625" style="14"/>
   </cols>
   <sheetData>
@@ -2234,7 +2234,7 @@
         <v>26</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>295</v>
@@ -2290,13 +2290,13 @@
         <v>32</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>284</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
         <v>38</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
@@ -2453,13 +2453,13 @@
         <v>38</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>285</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2510,7 +2510,7 @@
         <v>38</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -2553,7 +2553,7 @@
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>25</v>
@@ -2565,7 +2565,7 @@
         <v>38</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -2755,7 +2755,7 @@
         <v>38</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -2802,7 +2802,7 @@
         <v>58</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R13" s="14" t="s">
         <v>58</v>
@@ -2861,7 +2861,7 @@
         <v>38</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -3008,7 +3008,7 @@
         <v>32</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -3108,7 +3108,7 @@
         <v>32</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -3204,7 +3204,7 @@
         <v>88</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>25</v>
@@ -3216,7 +3216,7 @@
         <v>32</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -3263,7 +3263,7 @@
         <v>32</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -3367,7 +3367,7 @@
         <v>32</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
@@ -3412,7 +3412,7 @@
         <v>113</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>25</v>
@@ -3424,13 +3424,13 @@
         <v>32</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T25" s="8" t="s">
         <v>334</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -3471,7 +3471,7 @@
         <v>113</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>25</v>
@@ -3483,13 +3483,13 @@
         <v>32</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T26" s="8" t="s">
         <v>334</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -3530,7 +3530,7 @@
         <v>340</v>
       </c>
       <c r="O27" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>25</v>
@@ -3542,7 +3542,7 @@
         <v>32</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
@@ -3572,18 +3572,18 @@
       <c r="H28" s="1"/>
       <c r="I28" s="12"/>
       <c r="J28" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="M28" s="12"/>
       <c r="N28" s="1"/>
       <c r="O28" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>25</v>
@@ -3595,13 +3595,13 @@
         <v>32</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="T28" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -3643,16 +3643,16 @@
         <v>26</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="S29" s="1">
         <v>2</v>
       </c>
       <c r="T29" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -3727,13 +3727,13 @@
       <c r="H31" s="1"/>
       <c r="I31" s="12"/>
       <c r="J31" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="K31" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="M31" s="12"/>
       <c r="N31" s="1" t="s">
@@ -3780,13 +3780,13 @@
       <c r="H32" s="1"/>
       <c r="I32" s="12"/>
       <c r="J32" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>351</v>
       </c>
       <c r="M32" s="12"/>
       <c r="N32" s="1" t="s">
@@ -3836,10 +3836,10 @@
         <v>292</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M33" s="12"/>
       <c r="N33" s="1" t="s">
@@ -3889,10 +3889,10 @@
         <v>293</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M34" s="12"/>
       <c r="N34" s="1" t="s">
@@ -3939,20 +3939,20 @@
       <c r="H35" s="1"/>
       <c r="I35" s="12"/>
       <c r="J35" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="K35" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="K35" s="7" t="s">
-        <v>355</v>
-      </c>
       <c r="L35" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M35" s="12"/>
       <c r="N35" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>25</v>
@@ -3964,7 +3964,7 @@
         <v>201</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
@@ -3994,13 +3994,13 @@
       <c r="H36" s="1"/>
       <c r="I36" s="12"/>
       <c r="J36" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="L36" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M36" s="12"/>
       <c r="N36" s="1" t="s">
@@ -4047,22 +4047,22 @@
       <c r="H37" s="1"/>
       <c r="I37" s="12"/>
       <c r="J37" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="M37" s="12" t="s">
         <v>361</v>
-      </c>
-      <c r="M37" s="12" t="s">
-        <v>362</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>145</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>25</v>
@@ -4079,7 +4079,7 @@
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4104,16 +4104,16 @@
       <c r="H38" s="1"/>
       <c r="I38" s="12"/>
       <c r="J38" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>367</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>149</v>
@@ -4129,7 +4129,7 @@
         <v>201</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="U38" s="1"/>
     </row>
@@ -4180,7 +4180,7 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
     </row>
-    <row r="40" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4205,16 +4205,16 @@
       <c r="H40" s="1"/>
       <c r="I40" s="12"/>
       <c r="J40" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="L40" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="M40" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>367</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>149</v>
@@ -4230,7 +4230,7 @@
         <v>201</v>
       </c>
       <c r="S40" s="7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
@@ -4307,16 +4307,16 @@
       <c r="H42" s="1"/>
       <c r="I42" s="12"/>
       <c r="J42" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="M42" s="12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>162</v>
@@ -4362,16 +4362,16 @@
       <c r="H43" s="1"/>
       <c r="I43" s="12"/>
       <c r="J43" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="K43" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="L43" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="M43" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="M43" s="12" t="s">
-        <v>367</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>149</v>
@@ -4387,7 +4387,7 @@
         <v>32</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
@@ -4464,16 +4464,16 @@
         <v>173</v>
       </c>
       <c r="J45" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="12" t="s">
         <v>378</v>
-      </c>
-      <c r="M45" s="12" t="s">
-        <v>379</v>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -4487,7 +4487,7 @@
         <v>38</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
@@ -4517,16 +4517,16 @@
         <v>176</v>
       </c>
       <c r="J46" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="12" t="s">
         <v>378</v>
-      </c>
-      <c r="M46" s="12" t="s">
-        <v>379</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -4616,16 +4616,16 @@
         <v>182</v>
       </c>
       <c r="J48" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="12" t="s">
         <v>383</v>
-      </c>
-      <c r="M48" s="12" t="s">
-        <v>384</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -4669,19 +4669,19 @@
         <v>186</v>
       </c>
       <c r="J49" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K49" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="M49" s="12" t="s">
+      <c r="O49" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>25</v>
@@ -4693,7 +4693,7 @@
         <v>38</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
@@ -4770,16 +4770,16 @@
         <v>186</v>
       </c>
       <c r="J51" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="K51" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="M51" s="12" t="s">
         <v>393</v>
-      </c>
-      <c r="M51" s="12" t="s">
-        <v>394</v>
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -4793,7 +4793,7 @@
         <v>38</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
@@ -4823,16 +4823,16 @@
         <v>194</v>
       </c>
       <c r="J52" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="M52" s="12" t="s">
         <v>393</v>
-      </c>
-      <c r="M52" s="12" t="s">
-        <v>394</v>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -4846,7 +4846,7 @@
         <v>38</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
@@ -4970,16 +4970,16 @@
         <v>186</v>
       </c>
       <c r="J55" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="K55" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="M55" s="12" t="s">
         <v>399</v>
-      </c>
-      <c r="M55" s="12" t="s">
-        <v>400</v>
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -5023,16 +5023,16 @@
         <v>186</v>
       </c>
       <c r="J56" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="K56" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>402</v>
-      </c>
       <c r="L56" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="M56" s="12" t="s">
         <v>399</v>
-      </c>
-      <c r="M56" s="12" t="s">
-        <v>400</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -5076,16 +5076,16 @@
         <v>186</v>
       </c>
       <c r="J57" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="K57" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="K57" s="6" t="s">
-        <v>404</v>
-      </c>
       <c r="L57" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="M57" s="13" t="s">
         <v>399</v>
-      </c>
-      <c r="M57" s="13" t="s">
-        <v>400</v>
       </c>
       <c r="N57" s="6"/>
       <c r="O57" s="1"/>
@@ -5354,16 +5354,16 @@
       <c r="H63" s="1"/>
       <c r="I63" s="12"/>
       <c r="J63" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="K63" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="K63" s="7" t="s">
+      <c r="L63" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="L63" s="1" t="s">
+      <c r="M63" s="12" t="s">
         <v>407</v>
-      </c>
-      <c r="M63" s="12" t="s">
-        <v>408</v>
       </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
@@ -5377,7 +5377,7 @@
         <v>32</v>
       </c>
       <c r="S63" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
@@ -6225,7 +6225,7 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
     </row>
-    <row r="82" spans="1:21" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="57" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -6250,19 +6250,19 @@
         <v>186</v>
       </c>
       <c r="J82" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="K82" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="L82" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="L82" s="1" t="s">
+      <c r="M82" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="N82" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="M82" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="N82" s="1" t="s">
-        <v>413</v>
       </c>
       <c r="O82" s="1"/>
       <c r="P82" s="1" t="s">
@@ -6275,12 +6275,12 @@
         <v>201</v>
       </c>
       <c r="S82" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
     </row>
-    <row r="83" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" ht="199.5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -6303,16 +6303,16 @@
       <c r="H83" s="1"/>
       <c r="I83" s="12"/>
       <c r="J83" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="L83" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="K83" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="L83" s="1" t="s">
+      <c r="M83" s="12" t="s">
         <v>416</v>
-      </c>
-      <c r="M83" s="12" t="s">
-        <v>417</v>
       </c>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
@@ -6326,12 +6326,12 @@
         <v>32</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
     </row>
-    <row r="84" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -6356,12 +6356,12 @@
       <c r="H84" s="1"/>
       <c r="I84" s="12"/>
       <c r="J84" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
       <c r="M84" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
@@ -6375,7 +6375,7 @@
         <v>32</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>

</xml_diff>

<commit_message>
Correct valuetype fruit and vegetable quantity
</commit_message>
<xml_diff>
--- a/data_processing_elements-MSN.xlsx
+++ b/data_processing_elements-MSN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B02D24-1CFC-406F-BEBE-E43F86252165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58D95AF-FB99-4211-A9AC-D9779696A3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -2105,10 +2105,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P84" sqref="P84"/>
+      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4103,7 +4103,7 @@
         <v>148</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>149</v>
@@ -4204,7 +4204,7 @@
         <v>156</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
correct vegetable and fruit quantity harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-MSN.xlsx
+++ b/data_processing_elements-MSN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58D95AF-FB99-4211-A9AC-D9779696A3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3B9B4B-DF8E-4662-8588-5C1A03B9CB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1572,16 +1572,6 @@
 ELSE ~ NA_real_)</t>
   </si>
   <si>
-    <t>case_when(
-fruit_total &gt;= 0 ~ as.integer(round(fruit_total, 0)); 
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
-    <t>case_when(
-fruit_total &gt;= 0 ~ as.integer(round(vegetables_total, 0)); 
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>round((13.895 * N_Wmax_combined + 151) / Weight, 2)</t>
   </si>
   <si>
@@ -1603,6 +1593,16 @@
                            temp_SF36_Q08, temp_SF36_Q09, temp_SF36_Q10, temp_SF36_Q11, temp_SF36_Q12),
                 na.rm=TRUE)) %&gt;%
 mutate(phy_SF36_nb_items = if_else(phy_SF36_nb_items == 0, NA, phy_SF36_nb_items)</t>
+  </si>
+  <si>
+    <t>case_when(
+fruit_total &gt;= 0 ~ fruit_total; 
+ELSE ~ NA_real_)</t>
+  </si>
+  <si>
+    <t>case_when(
+fruit_total &gt;= 0 ~ vegetables_total; 
+ELSE ~ NA_real_)</t>
   </si>
 </sst>
 </file>
@@ -2105,10 +2105,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3579,7 +3579,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="10"/>
       <c r="J28" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>341</v>
@@ -3602,7 +3602,7 @@
         <v>32</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="T28" s="7" t="s">
         <v>343</v>
@@ -4086,7 +4086,7 @@
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4135,8 +4135,8 @@
       <c r="R38" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="S38" s="1" t="s">
-        <v>450</v>
+      <c r="S38" s="17" t="s">
+        <v>453</v>
       </c>
       <c r="U38" s="1"/>
     </row>
@@ -4187,7 +4187,7 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4236,8 +4236,8 @@
       <c r="R40" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="S40" s="1" t="s">
-        <v>451</v>
+      <c r="S40" s="17" t="s">
+        <v>454</v>
       </c>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
@@ -6382,7 +6382,7 @@
         <v>32</v>
       </c>
       <c r="S84" s="17" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="T84" s="18"/>
       <c r="U84" s="1"/>

</xml_diff>